<commit_message>
Centralized hash function in utility and made sure flags in hashstr are sorted in case they are a different order, which would result in a different hash
</commit_message>
<xml_diff>
--- a/results/results_formatted.xlsx
+++ b/results/results_formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Yuman\Desktop\MasterProject\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{080CB5BA-2629-406A-A55B-373C3C2D2E58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C47D11E-735E-4D79-9304-9634A2CE9C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
   <si>
     <t>ID</t>
   </si>
@@ -53,6 +53,129 @@
   </si>
   <si>
     <t>HASH</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>C</t>
+  </si>
+  <si>
+    <t>GO</t>
+  </si>
+  <si>
+    <t>achiral_catalyst</t>
+  </si>
+  <si>
+    <t>Cl</t>
+  </si>
+  <si>
+    <t>Br</t>
+  </si>
+  <si>
+    <t>Rsub</t>
+  </si>
+  <si>
+    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\1.achiral_catalyst.Cl_Br_ZnCl2.Rsub</t>
+  </si>
+  <si>
+    <t>GO R2=Br R1=Cl</t>
+  </si>
+  <si>
+    <t>1b962d1743668d385c13ad4396082534c8cbd0d04bd43bb91a4b23893134d0ac</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>Rrad</t>
+  </si>
+  <si>
+    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\2.achiral_catalyst.Cl_Br_ZnCl2.Rrad</t>
+  </si>
+  <si>
+    <t>GO radical</t>
+  </si>
+  <si>
+    <t>08fba8608791072397dd60e4fb75c6e912314dd0dd533f9b3b0e13a505ff3f51</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>ZnCl2</t>
+  </si>
+  <si>
+    <t>Rcat</t>
+  </si>
+  <si>
+    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\3.achiral_catalyst.Cl_Br_ZnCl2.Rcat</t>
+  </si>
+  <si>
+    <t>GO Rcat=ZnCl2</t>
+  </si>
+  <si>
+    <t>ebb568b4f698b5736b1af496c81569623796e1a6889795223b427f76f3d36e2f</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Rsub_cat_complex</t>
+  </si>
+  <si>
+    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\4.achiral_catalyst.Cl_Br_ZnCl2.Rsub_cat_complex</t>
+  </si>
+  <si>
+    <t>GO R2=Br R1=Cl Rcat=ZnCl2</t>
+  </si>
+  <si>
+    <t>663b22395aad2cc9df8e90353306f288b067f306f701f41801afc2610f521dcb</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>TSRC</t>
+  </si>
+  <si>
+    <t>TS</t>
+  </si>
+  <si>
+    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\5.achiral_catalyst.Cl_Br_ZnCl2.TS</t>
+  </si>
+  <si>
+    <t>TSRC radical TSRC=2_10 R2=Br R1=Cl Rcat=ZnCl2</t>
+  </si>
+  <si>
+    <t>8b76f718118c233334705d3590c5a8eea2cf9b7a0bc6161905836bd905f6f045</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>P1</t>
+  </si>
+  <si>
+    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\6.achiral_catalyst.Cl_Br_ZnCl2.P1</t>
+  </si>
+  <si>
+    <t>GO radical R2=Br R1=Cl Rcat=ZnCl2</t>
+  </si>
+  <si>
+    <t>c86ba910299a0686ac87544a813d7647897ccead1ef51625fdb2898e9ca69351</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>P2</t>
+  </si>
+  <si>
+    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\7.achiral_catalyst.Cl_Br_ZnCl2.P2</t>
+  </si>
+  <si>
+    <t>33cbe882b5288e1a0a33dc017eebab74057b0bc6cec40fd82c8eccdb69e6691d</t>
   </si>
 </sst>
 </file>
@@ -68,12 +191,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF898989"/>
+        <bgColor rgb="FF898989"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -88,8 +217,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -392,7 +522,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:K8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -401,13 +531,13 @@
     <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="5.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="68.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
@@ -445,6 +575,239 @@
         <v>10</v>
       </c>
     </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="1"/>
+      <c r="H3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
+      <c r="G4" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Progress on Excel formatter. Added links to DIRECTORY and added bat script to run molviewer2 to show geometries of jobs. Also added freezepanes for top row and first column
</commit_message>
<xml_diff>
--- a/results/results_formatted.xlsx
+++ b/results/results_formatted.xlsx
@@ -8,19 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Yuman\Desktop\MasterProject\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C47D11E-735E-4D79-9304-9634A2CE9C8C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB866F48-CD4C-4162-9BBE-1D7CDD5A9027}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2850" yWindow="2850" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Overview" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Overview!$A$1:$L$8</definedName>
+  </definedNames>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="46">
   <si>
     <t>ID</t>
   </si>
@@ -52,6 +66,9 @@
     <t>FLAGS</t>
   </si>
   <si>
+    <t>GEOMETRY</t>
+  </si>
+  <si>
     <t>HASH</t>
   </si>
   <si>
@@ -76,9 +93,6 @@
     <t>Rsub</t>
   </si>
   <si>
-    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\1.achiral_catalyst.Cl_Br_ZnCl2.Rsub</t>
-  </si>
-  <si>
     <t>GO R2=Br R1=Cl</t>
   </si>
   <si>
@@ -91,9 +105,6 @@
     <t>Rrad</t>
   </si>
   <si>
-    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\2.achiral_catalyst.Cl_Br_ZnCl2.Rrad</t>
-  </si>
-  <si>
     <t>GO radical</t>
   </si>
   <si>
@@ -109,9 +120,6 @@
     <t>Rcat</t>
   </si>
   <si>
-    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\3.achiral_catalyst.Cl_Br_ZnCl2.Rcat</t>
-  </si>
-  <si>
     <t>GO Rcat=ZnCl2</t>
   </si>
   <si>
@@ -124,9 +132,6 @@
     <t>Rsub_cat_complex</t>
   </si>
   <si>
-    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\4.achiral_catalyst.Cl_Br_ZnCl2.Rsub_cat_complex</t>
-  </si>
-  <si>
     <t>GO R2=Br R1=Cl Rcat=ZnCl2</t>
   </si>
   <si>
@@ -142,9 +147,6 @@
     <t>TS</t>
   </si>
   <si>
-    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\5.achiral_catalyst.Cl_Br_ZnCl2.TS</t>
-  </si>
-  <si>
     <t>TSRC radical TSRC=2_10 R2=Br R1=Cl Rcat=ZnCl2</t>
   </si>
   <si>
@@ -157,9 +159,6 @@
     <t>P1</t>
   </si>
   <si>
-    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\6.achiral_catalyst.Cl_Br_ZnCl2.P1</t>
-  </si>
-  <si>
     <t>GO radical R2=Br R1=Cl Rcat=ZnCl2</t>
   </si>
   <si>
@@ -170,9 +169,6 @@
   </si>
   <si>
     <t>P2</t>
-  </si>
-  <si>
-    <t>calculations\achiral_catalyst_Cl_Br_ZnCl2\7.achiral_catalyst.Cl_Br_ZnCl2.P2</t>
   </si>
   <si>
     <t>33cbe882b5288e1a0a33dc017eebab74057b0bc6cec40fd82c8eccdb69e6691d</t>
@@ -182,10 +178,22 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -200,12 +208,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF898989"/>
-        <bgColor rgb="FF898989"/>
+        <fgColor rgb="FFDBDBDB"/>
+        <bgColor rgb="FFDBDBDB"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -213,15 +221,44 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -522,293 +559,320 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K8"/>
+  <dimension ref="A1:L8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight"/>
+      <selection pane="bottomLeft"/>
+      <selection pane="bottomRight"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="7.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="3.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="5.85546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="83.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="5.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="7.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="90.28515625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="43.140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="68.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.28515625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="68.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="K1" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="L1" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="2" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="B2" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="C2" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D2" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="E2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="G2" s="1"/>
-      <c r="H2" s="1" t="s">
+      <c r="F2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="I2" s="1" t="s">
+      <c r="G2" s="3"/>
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="J2" s="1" t="s">
+      <c r="I2" s="4" t="str">
+        <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\calculations\achiral_catalyst_Cl_Br_ZnCl2\1.achiral_catalyst.Cl_Br_ZnCl2.Rsub", "calculations\achiral_catalyst_Cl_Br_ZnCl2\1.achiral_catalyst.Cl_Br_ZnCl2.Rsub")</f>
+        <v>calculations\achiral_catalyst_Cl_Br_ZnCl2\1.achiral_catalyst.Cl_Br_ZnCl2.Rsub</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="K2" s="1" t="s">
+      <c r="K2" s="3"/>
+      <c r="L2" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E3" s="1"/>
-      <c r="F3" s="1"/>
-      <c r="G3" s="1"/>
-      <c r="H3" s="1" t="s">
+      <c r="D3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="I3" s="4" t="str">
+        <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\calculations\achiral_catalyst_Cl_Br_ZnCl2\2.achiral_catalyst.Cl_Br_ZnCl2.Rrad", "calculations\achiral_catalyst_Cl_Br_ZnCl2\2.achiral_catalyst.Cl_Br_ZnCl2.Rrad")</f>
+        <v>calculations\achiral_catalyst_Cl_Br_ZnCl2\2.achiral_catalyst.Cl_Br_ZnCl2.Rrad</v>
+      </c>
+      <c r="J3" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="3"/>
+      <c r="L3" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="K3" s="1" t="s">
+    </row>
+    <row r="4" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>25</v>
       </c>
+      <c r="B4" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E4" s="3"/>
+      <c r="F4" s="3"/>
+      <c r="G4" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="I4" s="4" t="str">
+        <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\calculations\achiral_catalyst_Cl_Br_ZnCl2\3.achiral_catalyst.Cl_Br_ZnCl2.Rcat", "calculations\achiral_catalyst_Cl_Br_ZnCl2\3.achiral_catalyst.Cl_Br_ZnCl2.Rcat")</f>
+        <v>calculations\achiral_catalyst_Cl_Br_ZnCl2\3.achiral_catalyst.Cl_Br_ZnCl2.Rcat</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K4" s="4" t="str">
+        <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\calculations\achiral_catalyst_Cl_Br_ZnCl2\3.achiral_catalyst.Cl_Br_ZnCl2.Rcat/molview2_start.bat", "output.xyz")</f>
+        <v>output.xyz</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>29</v>
+      </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
+    <row r="5" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G5" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="H5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I5" s="4" t="str">
+        <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\calculations\achiral_catalyst_Cl_Br_ZnCl2\4.achiral_catalyst.Cl_Br_ZnCl2.Rsub_cat_complex", "calculations\achiral_catalyst_Cl_Br_ZnCl2\4.achiral_catalyst.Cl_Br_ZnCl2.Rsub_cat_complex")</f>
+        <v>calculations\achiral_catalyst_Cl_Br_ZnCl2\4.achiral_catalyst.Cl_Br_ZnCl2.Rsub_cat_complex</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="L5" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C6" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="I6" s="4" t="str">
+        <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\calculations\achiral_catalyst_Cl_Br_ZnCl2\5.achiral_catalyst.Cl_Br_ZnCl2.TS", "calculations\achiral_catalyst_Cl_Br_ZnCl2\5.achiral_catalyst.Cl_Br_ZnCl2.TS")</f>
+        <v>calculations\achiral_catalyst_Cl_Br_ZnCl2\5.achiral_catalyst.Cl_Br_ZnCl2.TS</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="L6" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="1"/>
-      <c r="F4" s="1"/>
-      <c r="G4" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>29</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" s="1" t="s">
-        <v>31</v>
+      <c r="D7" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I7" s="4" t="str">
+        <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\calculations\achiral_catalyst_Cl_Br_ZnCl2\6.achiral_catalyst.Cl_Br_ZnCl2.P1", "calculations\achiral_catalyst_Cl_Br_ZnCl2\6.achiral_catalyst.Cl_Br_ZnCl2.P1")</f>
+        <v>calculations\achiral_catalyst_Cl_Br_ZnCl2\6.achiral_catalyst.Cl_Br_ZnCl2.P1</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="L7" s="3" t="s">
+        <v>42</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
+    <row r="8" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="I8" s="4" t="str">
+        <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\calculations\achiral_catalyst_Cl_Br_ZnCl2\7.achiral_catalyst.Cl_Br_ZnCl2.P2", "calculations\achiral_catalyst_Cl_Br_ZnCl2\7.achiral_catalyst.Cl_Br_ZnCl2.P2")</f>
+        <v>calculations\achiral_catalyst_Cl_Br_ZnCl2\7.achiral_catalyst.Cl_Br_ZnCl2.P2</v>
+      </c>
+      <c r="J8" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B5" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="I7" s="1" t="s">
+      <c r="K8" s="3"/>
+      <c r="L8" s="3" t="s">
         <v>45</v>
-      </c>
-      <c r="J7" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C8" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>50</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K8" s="1" t="s">
-        <v>51</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:L8" xr:uid="{00000000-0009-0000-0000-000000000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Started work on squaramide templates
</commit_message>
<xml_diff>
--- a/results/results_formatted.xlsx
+++ b/results/results_formatted.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\Yuman\Desktop\MasterProject\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8F6C05A-5DFD-4A2B-BBFA-8B5CFB868539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67D20909-1A2A-416A-8DB8-D84A45B3A75D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7200" yWindow="2085" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="366" uniqueCount="93">
   <si>
     <t>STATUS</t>
   </si>
@@ -108,7 +108,10 @@
     <t>P1R_cat_complex</t>
   </si>
   <si>
-    <t>01:02:14</t>
+    <t>01:41:29</t>
+  </si>
+  <si>
+    <t>FREQ</t>
   </si>
   <si>
     <t>b0693f9e631444c871412593fa38a05a3f3050d558f7fcd345cdb2eab5804325</t>
@@ -120,10 +123,7 @@
     <t>P1S_cat_complex</t>
   </si>
   <si>
-    <t>00:12:42</t>
-  </si>
-  <si>
-    <t>FREQ</t>
+    <t>12:59:01</t>
   </si>
   <si>
     <t>1d05fa7c4170fed4d1e730d6a758699748b45993146d071df4316fb129a063db</t>
@@ -138,7 +138,7 @@
     <t>P2</t>
   </si>
   <si>
-    <t>01:12:20</t>
+    <t>01:12:19</t>
   </si>
   <si>
     <t>f33894258c9f3a01f4d0f3379ad3f5caa65e7dc17262bc674c20cf9ae9820576</t>
@@ -147,7 +147,7 @@
     <t>P2R_cat_complex</t>
   </si>
   <si>
-    <t>04:18:12</t>
+    <t>09:24:24</t>
   </si>
   <si>
     <t>24b8aabce8f736356e1624f9901f8ca2bcc9d93c3063a32b9bea69b5f5445fa0</t>
@@ -156,7 +156,7 @@
     <t>P2S_cat_complex</t>
   </si>
   <si>
-    <t>00:29:26</t>
+    <t>03:56:23</t>
   </si>
   <si>
     <t>729943bcad94f65100b4595220267912b8f018b697c3b78d710d9f7e4af500a0</t>
@@ -171,30 +171,36 @@
     <t>8e0bbd79aeb04fd96a9320a54ef7f4bfd7649e7c48c7cfc310460ea97618129d</t>
   </si>
   <si>
+    <t>sub_cat_complex</t>
+  </si>
+  <si>
+    <t>02:19:23</t>
+  </si>
+  <si>
+    <t>34149c4d9f34bf84857c3659209f0d409157db958fce6e8cb44481504eff37a5</t>
+  </si>
+  <si>
+    <t>TSRC</t>
+  </si>
+  <si>
+    <t>TSR</t>
+  </si>
+  <si>
+    <t>05:53:39</t>
+  </si>
+  <si>
+    <t>a6a67698b100f73fdf209512bf318ce3248429f6b6e9269ca7f356bf4eceac60</t>
+  </si>
+  <si>
     <t>Queued</t>
   </si>
   <si>
-    <t>sub_cat_complex</t>
+    <t>TSS</t>
   </si>
   <si>
     <t>00:00:00</t>
   </si>
   <si>
-    <t>34149c4d9f34bf84857c3659209f0d409157db958fce6e8cb44481504eff37a5</t>
-  </si>
-  <si>
-    <t>TSRC</t>
-  </si>
-  <si>
-    <t>TSR</t>
-  </si>
-  <si>
-    <t>a6a67698b100f73fdf209512bf318ce3248429f6b6e9269ca7f356bf4eceac60</t>
-  </si>
-  <si>
-    <t>TSS</t>
-  </si>
-  <si>
     <t>ae0494b902b29473ed0606c62b6871cd73bfc8d22c0af18a3ac88b934f0c67e2</t>
   </si>
   <si>
@@ -234,55 +240,55 @@
     <t>tBu</t>
   </si>
   <si>
-    <t>00:44:01</t>
+    <t>16:07:29</t>
   </si>
   <si>
     <t>866987efab919431232b933eceb7c714f097a87262498acab50ed9e1ef931fa4</t>
   </si>
   <si>
-    <t>00:19:18</t>
+    <t>12:33:18</t>
   </si>
   <si>
     <t>711f58f8bd073be0a3ad18c26d1f94ea62e79faff83f82f13e681b8cbdbad4b2</t>
   </si>
   <si>
-    <t>01:42:29</t>
+    <t>01:42:28</t>
   </si>
   <si>
     <t>09c16c2cea11ada970257b14275bd17b2415f1f5d88c8d0ba5c18d94ebfee162</t>
   </si>
   <si>
-    <t>39:43:02</t>
+    <t>15:43:02</t>
   </si>
   <si>
     <t>233b7088370e290dff760ab2a0eda7a94fa5711644602e33236324972af825f2</t>
   </si>
   <si>
-    <t>37:29:52</t>
+    <t>13:29:51</t>
   </si>
   <si>
     <t>4004637466a693ab01b82b43f533df53e7636e00dbc73963e11d1abd982e01a1</t>
   </si>
   <si>
-    <t>00:45:00</t>
+    <t>00:44:59</t>
   </si>
   <si>
     <t>178a71eb8aaa014318a096a3f978fe2aaaccc1b5f98b83ee03574a7425697aa4</t>
   </si>
   <si>
-    <t>27:44:20</t>
+    <t>03:44:20</t>
   </si>
   <si>
     <t>795a7056323637ae37f7063645b8be804046616041138aa6b537d8ac2d15475b</t>
   </si>
   <si>
-    <t>00:57:05</t>
+    <t>18:47:34</t>
   </si>
   <si>
     <t>f788c728429e1cfe5c4261ba72629fcdfb602c2225e4de93b74fe5aa20f8431c</t>
   </si>
   <si>
-    <t>01:00:50</t>
+    <t>16:01:16</t>
   </si>
   <si>
     <t>d5bd7f7f3a8a4925ee56ac66041fea0e2ffa6a5001bcf18ecf535ed2ca6da602</t>
@@ -846,10 +852,10 @@
         <v>24</v>
       </c>
       <c r="O2" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="P2" s="3" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -863,7 +869,7 @@
         <v>18</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>20</v>
@@ -876,7 +882,7 @@
         <v>22</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J3" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_O.vacuum\P1S_cat_complex", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_O.vacuum\P1S_cat_complex")</f>
@@ -889,10 +895,10 @@
       </c>
       <c r="M3" s="3"/>
       <c r="N3" s="5" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="O3" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P3" s="3" t="s">
         <v>30</v>
@@ -936,7 +942,7 @@
         <v>34</v>
       </c>
       <c r="O4" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>35</v>
@@ -982,7 +988,7 @@
         <v>37</v>
       </c>
       <c r="O5" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P5" s="3" t="s">
         <v>38</v>
@@ -999,7 +1005,7 @@
         <v>18</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>20</v>
@@ -1028,7 +1034,7 @@
         <v>40</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>41</v>
@@ -1072,15 +1078,15 @@
         <v>43</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P7" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="7" t="s">
-        <v>45</v>
+      <c r="A8" s="2" t="s">
+        <v>16</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>17</v>
@@ -1102,7 +1108,7 @@
         <v>22</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_O.vacuum\sub_cat_complex", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_O.vacuum\sub_cat_complex")</f>
@@ -1115,19 +1121,21 @@
       </c>
       <c r="M8" s="3"/>
       <c r="N8" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3" t="s">
+    </row>
+    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>48</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="7" t="s">
-        <v>45</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>18</v>
@@ -1146,7 +1154,7 @@
         <v>22</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J9" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_O.vacuum\TSR", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_O.vacuum\TSR")</f>
@@ -1159,25 +1167,27 @@
       </c>
       <c r="M9" s="3"/>
       <c r="N9" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="O9" s="3"/>
+        <v>50</v>
+      </c>
+      <c r="O9" s="3" t="s">
+        <v>17</v>
+      </c>
       <c r="P9" s="3" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>20</v>
@@ -1190,7 +1200,7 @@
         <v>22</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J10" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_O.vacuum\TSS", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_O.vacuum\TSS")</f>
@@ -1203,16 +1213,16 @@
       </c>
       <c r="M10" s="3"/>
       <c r="N10" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O10" s="3"/>
       <c r="P10" s="3" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>17</v>
@@ -1227,10 +1237,10 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
       <c r="H11" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J11" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\cat", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\cat")</f>
@@ -1243,16 +1253,16 @@
       </c>
       <c r="M11" s="3"/>
       <c r="N11" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O11" s="3"/>
       <c r="P11" s="3" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
     </row>
     <row r="12" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>17</v>
@@ -1271,7 +1281,7 @@
       </c>
       <c r="G12" s="3"/>
       <c r="H12" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I12" s="3" t="s">
         <v>23</v>
@@ -1287,16 +1297,16 @@
       </c>
       <c r="M12" s="3"/>
       <c r="N12" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O12" s="3"/>
       <c r="P12" s="3" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
     </row>
     <row r="13" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B13" s="3" t="s">
         <v>17</v>
@@ -1305,7 +1315,7 @@
         <v>18</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>20</v>
@@ -1315,10 +1325,10 @@
       </c>
       <c r="G13" s="3"/>
       <c r="H13" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I13" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J13" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\P1S_cat_complex", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\P1S_cat_complex")</f>
@@ -1331,16 +1341,16 @@
       </c>
       <c r="M13" s="3"/>
       <c r="N13" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O13" s="3"/>
       <c r="P13" s="3" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>17</v>
@@ -1359,7 +1369,7 @@
       </c>
       <c r="G14" s="3"/>
       <c r="H14" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I14" s="3" t="s">
         <v>36</v>
@@ -1375,16 +1385,16 @@
       </c>
       <c r="M14" s="3"/>
       <c r="N14" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O14" s="3"/>
       <c r="P14" s="3" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
     </row>
     <row r="15" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>17</v>
@@ -1393,7 +1403,7 @@
         <v>18</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>20</v>
@@ -1403,7 +1413,7 @@
       </c>
       <c r="G15" s="3"/>
       <c r="H15" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I15" s="3" t="s">
         <v>39</v>
@@ -1419,16 +1429,16 @@
       </c>
       <c r="M15" s="3"/>
       <c r="N15" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O15" s="3"/>
       <c r="P15" s="3" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
     </row>
     <row r="16" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>17</v>
@@ -1447,10 +1457,10 @@
       </c>
       <c r="G16" s="3"/>
       <c r="H16" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I16" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J16" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\sub_cat_complex", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\sub_cat_complex")</f>
@@ -1463,19 +1473,19 @@
       </c>
       <c r="M16" s="3"/>
       <c r="N16" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O16" s="3"/>
       <c r="P16" s="3" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C17" s="3" t="s">
         <v>18</v>
@@ -1491,10 +1501,10 @@
       </c>
       <c r="G17" s="3"/>
       <c r="H17" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I17" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J17" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\TSR", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\TSR")</f>
@@ -1507,25 +1517,25 @@
       </c>
       <c r="M17" s="3"/>
       <c r="N17" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O17" s="3"/>
       <c r="P17" s="3" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
     </row>
     <row r="18" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>20</v>
@@ -1535,10 +1545,10 @@
       </c>
       <c r="G18" s="3"/>
       <c r="H18" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I18" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J18" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\TSS", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_Ph_S.vacuum\TSS")</f>
@@ -1551,11 +1561,11 @@
       </c>
       <c r="M18" s="3"/>
       <c r="N18" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O18" s="3"/>
       <c r="P18" s="3" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="19" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1578,7 +1588,7 @@
         <v>22</v>
       </c>
       <c r="I19" s="3" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="J19" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\cat", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\cat")</f>
@@ -1591,18 +1601,18 @@
       </c>
       <c r="M19" s="3"/>
       <c r="N19" s="5" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="O19" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P19" s="3" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
     </row>
     <row r="20" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A20" s="2" t="s">
-        <v>16</v>
+      <c r="A20" s="6" t="s">
+        <v>31</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>17</v>
@@ -1617,7 +1627,7 @@
         <v>20</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G20" s="3"/>
       <c r="H20" s="3" t="s">
@@ -1637,40 +1647,40 @@
       </c>
       <c r="M20" s="3"/>
       <c r="N20" s="5" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="O20" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P20" s="3" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F21" s="3" t="s">
         <v>67</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A21" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>65</v>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I21" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J21" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\P1S_cat_complex", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\P1S_cat_complex")</f>
@@ -1683,13 +1693,13 @@
       </c>
       <c r="M21" s="3"/>
       <c r="N21" s="5" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="O21" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P21" s="3" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
     </row>
     <row r="22" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1709,7 +1719,7 @@
         <v>20</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G22" s="3"/>
       <c r="H22" s="3"/>
@@ -1727,13 +1737,13 @@
       </c>
       <c r="M22" s="3"/>
       <c r="N22" s="5" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="O22" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P22" s="3" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
     </row>
     <row r="23" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1753,7 +1763,7 @@
         <v>20</v>
       </c>
       <c r="F23" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G23" s="3"/>
       <c r="H23" s="3" t="s">
@@ -1773,13 +1783,13 @@
       </c>
       <c r="M23" s="3"/>
       <c r="N23" s="5" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="O23" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P23" s="3" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1793,13 +1803,13 @@
         <v>18</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F24" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G24" s="3"/>
       <c r="H24" s="3" t="s">
@@ -1819,13 +1829,13 @@
       </c>
       <c r="M24" s="3"/>
       <c r="N24" s="5" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="O24" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P24" s="3" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
     </row>
     <row r="25" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1845,7 +1855,7 @@
         <v>20</v>
       </c>
       <c r="F25" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G25" s="3"/>
       <c r="H25" s="3"/>
@@ -1863,13 +1873,13 @@
       </c>
       <c r="M25" s="3"/>
       <c r="N25" s="5" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="O25" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P25" s="3" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="26" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1889,14 +1899,14 @@
         <v>20</v>
       </c>
       <c r="F26" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G26" s="3"/>
       <c r="H26" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I26" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J26" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\sub_cat_complex", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\sub_cat_complex")</f>
@@ -1909,13 +1919,13 @@
       </c>
       <c r="M26" s="3"/>
       <c r="N26" s="5" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="O26" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P26" s="3" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
     </row>
     <row r="27" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1923,7 +1933,7 @@
         <v>16</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C27" s="3" t="s">
         <v>18</v>
@@ -1935,14 +1945,14 @@
         <v>20</v>
       </c>
       <c r="F27" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G27" s="3"/>
       <c r="H27" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I27" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J27" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\TSR", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\TSR")</f>
@@ -1955,13 +1965,13 @@
       </c>
       <c r="M27" s="3"/>
       <c r="N27" s="5" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="O27" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P27" s="3" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
@@ -1969,26 +1979,26 @@
         <v>16</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C28" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G28" s="3"/>
       <c r="H28" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I28" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J28" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\TSS", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_O.vacuum\TSS")</f>
@@ -2001,18 +2011,18 @@
       </c>
       <c r="M28" s="3"/>
       <c r="N28" s="5" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="O28" s="3" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="P28" s="3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="29" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B29" s="3" t="s">
         <v>17</v>
@@ -2027,11 +2037,11 @@
         <v>20</v>
       </c>
       <c r="F29" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G29" s="3"/>
       <c r="H29" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I29" s="3" t="s">
         <v>23</v>
@@ -2047,16 +2057,16 @@
       </c>
       <c r="M29" s="3"/>
       <c r="N29" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O29" s="3"/>
       <c r="P29" s="3" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B30" s="3" t="s">
         <v>17</v>
@@ -2065,20 +2075,20 @@
         <v>18</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E30" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F30" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G30" s="3"/>
       <c r="H30" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I30" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="J30" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_S.vacuum\P1S_cat_complex", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_S.vacuum\P1S_cat_complex")</f>
@@ -2091,16 +2101,16 @@
       </c>
       <c r="M30" s="3"/>
       <c r="N30" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O30" s="3"/>
       <c r="P30" s="3" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
     </row>
     <row r="31" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B31" s="3" t="s">
         <v>17</v>
@@ -2115,11 +2125,11 @@
         <v>20</v>
       </c>
       <c r="F31" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G31" s="3"/>
       <c r="H31" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I31" s="3" t="s">
         <v>36</v>
@@ -2135,16 +2145,16 @@
       </c>
       <c r="M31" s="3"/>
       <c r="N31" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O31" s="3"/>
       <c r="P31" s="3" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B32" s="3" t="s">
         <v>17</v>
@@ -2153,17 +2163,17 @@
         <v>18</v>
       </c>
       <c r="D32" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F32" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G32" s="3"/>
       <c r="H32" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I32" s="3" t="s">
         <v>39</v>
@@ -2179,16 +2189,16 @@
       </c>
       <c r="M32" s="3"/>
       <c r="N32" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O32" s="3"/>
       <c r="P32" s="3" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
     </row>
     <row r="33" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B33" s="3" t="s">
         <v>17</v>
@@ -2203,14 +2213,14 @@
         <v>20</v>
       </c>
       <c r="F33" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G33" s="3"/>
       <c r="H33" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I33" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J33" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_S.vacuum\sub_cat_complex", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_S.vacuum\sub_cat_complex")</f>
@@ -2223,19 +2233,19 @@
       </c>
       <c r="M33" s="3"/>
       <c r="N33" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O33" s="3"/>
       <c r="P33" s="3" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
     </row>
     <row r="34" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B34" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C34" s="3" t="s">
         <v>18</v>
@@ -2247,14 +2257,14 @@
         <v>20</v>
       </c>
       <c r="F34" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G34" s="3"/>
       <c r="H34" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I34" s="3" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="J34" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_S.vacuum\TSR", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_S.vacuum\TSR")</f>
@@ -2267,38 +2277,38 @@
       </c>
       <c r="M34" s="3"/>
       <c r="N34" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O34" s="3"/>
       <c r="P34" s="3" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="35" spans="1:16" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
-        <v>45</v>
+        <v>52</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>18</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>20</v>
       </c>
       <c r="F35" s="3" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G35" s="3"/>
       <c r="H35" s="3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I35" s="3" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="J35" s="4" t="str">
         <f>HYPERLINK("D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_S.vacuum\TSS", "D:\Users\Yuman\Desktop\MasterProject\results\urea_tBu_Ph.H_tBu_S.vacuum\TSS")</f>
@@ -2311,11 +2321,11 @@
       </c>
       <c r="M35" s="3"/>
       <c r="N35" s="5" t="s">
-        <v>47</v>
+        <v>54</v>
       </c>
       <c r="O35" s="3"/>
       <c r="P35" s="3" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>

</xml_diff>